<commit_message>
Atualizado layout de páginas e organização
</commit_message>
<xml_diff>
--- a/banco_dados/aulas_ministradas.xlsx
+++ b/banco_dados/aulas_ministradas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e3615100550b18e/Documentos/Projetos R/CursoExperimentacaoAgricolaR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marle\OneDrive\Documentos\Projetos R\site\banco_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="11_AD4D361C20488DEA4E38A0A4D4DD50005ADEDD81" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EFAD13E-E877-48D5-9B7C-617F46BFECB9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF370B2F-4C8D-431B-A435-2B442ACE5FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Aula</t>
   </si>
@@ -81,6 +81,19 @@
 Apresentação da interface do RStudio;
 Criação e salvamento do primeiro script;
 Definição do diretório de trabalho (working directory) (setwd(); getwd()).</t>
+  </si>
+  <si>
+    <t>Aula 3</t>
+  </si>
+  <si>
+    <t>Discussão sobre tipos de variáveis e desenho de experimentos.</t>
+  </si>
+  <si>
+    <t>Reconhecendo os tipos de variáveis no exerimento no Excel;
+Como organizar os dados no Excel;
+Entendo sobre variáveis dependentes e independentes;
+Entendendo sobre fatores e níveis de fatores;
+Discussão sobre desenho de experimento (simples e fatorial) e analises estatísticas (paramétrica, não-paramétrica, análise univariada, bivariada e multivariada).</t>
   </si>
 </sst>
 </file>
@@ -181,8 +194,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C071FD7A-8C48-4F93-B54C-3FE8AB0A6C8E}" name="Tabela1" displayName="Tabela1" ref="A1:G3" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G3" xr:uid="{C071FD7A-8C48-4F93-B54C-3FE8AB0A6C8E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C071FD7A-8C48-4F93-B54C-3FE8AB0A6C8E}" name="Tabela1" displayName="Tabela1" ref="A1:G4" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G4" xr:uid="{C071FD7A-8C48-4F93-B54C-3FE8AB0A6C8E}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{DDB91308-6503-4F02-A9E1-EDA751460085}" name="Aula" dataDxfId="6"/>
     <tableColumn id="7" xr3:uid="{49321207-4CF5-4BBD-B89D-B453F947217F}" name="Descrição" dataDxfId="5"/>
@@ -461,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,6 +565,30 @@
       </c>
       <c r="H3" s="4"/>
     </row>
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45910</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="F4" s="4">
+        <f>HOUR(Tabela1[[#This Row],[Horário de fim da aula]]-Tabela1[[#This Row],[Horário de nício da aula]])+(MINUTE(Tabela1[[#This Row],[Horário de fim da aula]]-Tabela1[[#This Row],[Horário de nício da aula]])/60)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>